<commit_message>
Updated macros to pull BOM font info, re-ran on Assign 3
</commit_message>
<xml_diff>
--- a/S2022_Tests/ASS_03_Testing/StudentFolder/Ex.1/ExcelExtract.xlsx
+++ b/S2022_Tests/ASS_03_Testing/StudentFolder/Ex.1/ExcelExtract.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\SolidWorks\AutoMARK\AutoMARK_V6\S2022_Tests\ASS_03_Testing\StudentFolder\Ex.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E21C3D8-82D7-4360-B86F-E13D748D431F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0A76CF8-6052-4A03-BD8D-05A16145C539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="953" yWindow="2847" windowWidth="13120" windowHeight="7660" xr2:uid="{3FC467D8-0E4D-434F-A2BE-F08E5C4BEED6}"/>
+    <workbookView xWindow="953" yWindow="2847" windowWidth="13120" windowHeight="7660" xr2:uid="{5D193994-C602-425A-9401-88C04CD99DDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1705,7 +1705,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1641468D-D34B-41D9-AF17-4A6684EC53B3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A205DF5A-9122-493C-8897-95DE5353CDD8}">
   <dimension ref="A1:AS344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>